<commit_message>
Adding dash to site pages
</commit_message>
<xml_diff>
--- a/static/excelsFiles/excelCountGenerally.xlsx
+++ b/static/excelsFiles/excelCountGenerally.xlsx
@@ -462,10 +462,10 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C2" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D2" t="n">
         <v>1</v>

</xml_diff>